<commit_message>
agregadas simulaciones - corregido error PCB
</commit_message>
<xml_diff>
--- a/EJ4/calculo_ganancia.xlsx
+++ b/EJ4/calculo_ganancia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joaco\Desktop\repos\TC\TP3\EJ4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F919605-2D03-48C2-A8A3-519F17F96887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D796DA68-DE07-4B7F-96E6-AEFCC46EA9E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{96CE2554-F54B-432E-AADA-E14654DB6005}"/>
+    <workbookView xWindow="14184" yWindow="5328" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{96CE2554-F54B-432E-AADA-E14654DB6005}"/>
   </bookViews>
   <sheets>
     <sheet name="mal" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>R1</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>SMD</t>
+  </si>
+  <si>
+    <t>68k</t>
   </si>
 </sst>
 </file>
@@ -741,7 +744,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,11 +882,13 @@
         <f t="shared" si="0"/>
         <v>1846.1538461538462</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="e">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G5" s="4" t="e">
         <f t="shared" si="2"/>

</xml_diff>